<commit_message>
formular to calculate shortfall
</commit_message>
<xml_diff>
--- a/uploads/stats_test.xlsx
+++ b/uploads/stats_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Work\altitudebpo_online_stats\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Work\altitudebpo_online_stats\Altitudebpo-online-dashboard\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87FD2487-B073-4953-8436-868155AFEE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18614F5-A6AB-41DE-B59B-824DDB2C3CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{8FFCB777-CAED-42EB-9B0B-CBE135F75017}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="15300" windowHeight="7785" xr2:uid="{8FFCB777-CAED-42EB-9B0B-CBE135F75017}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Team</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Current</t>
-  </si>
-  <si>
-    <t>Shortfall</t>
   </si>
   <si>
     <t>Team Glanton</t>
@@ -431,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131B74AE-0361-4281-8F46-2B4C27233B06}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +439,7 @@
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -452,50 +449,38 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" s="1">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="C2" s="1">
         <v>20</v>
       </c>
-      <c r="D2" s="1">
-        <v>40</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="C3" s="1">
         <v>20</v>
       </c>
-      <c r="D3" s="1">
-        <v>40</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="C4" s="1">
         <v>20</v>
-      </c>
-      <c r="D4" s="1">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
global totals-seperate user function
</commit_message>
<xml_diff>
--- a/uploads/stats_test.xlsx
+++ b/uploads/stats_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Work\altitudebpo_online_stats\Altitudebpo-online-dashboard\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18614F5-A6AB-41DE-B59B-824DDB2C3CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC08DEBE-6037-4F7E-86A3-E87A844DA235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="15300" windowHeight="7785" xr2:uid="{8FFCB777-CAED-42EB-9B0B-CBE135F75017}"/>
   </bookViews>
@@ -45,13 +45,13 @@
     <t>Current</t>
   </si>
   <si>
-    <t>Team Glanton</t>
-  </si>
-  <si>
-    <t>Team Tebogo</t>
-  </si>
-  <si>
-    <t>Team Victus</t>
+    <t>Team Pat</t>
+  </si>
+  <si>
+    <t>Team Themba</t>
+  </si>
+  <si>
+    <t>Team Sbu</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +458,7 @@
         <v>300</v>
       </c>
       <c r="C2" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>300</v>
       </c>
       <c r="C3" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>300</v>
       </c>
       <c r="C4" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new admin profile & breakdown stats button
</commit_message>
<xml_diff>
--- a/uploads/stats_test.xlsx
+++ b/uploads/stats_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Work\altitudebpo_online_stats\Altitudebpo-online-dashboard\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC08DEBE-6037-4F7E-86A3-E87A844DA235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DFA796-ECB9-4650-97A5-6437E21C0D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="15300" windowHeight="7785" xr2:uid="{8FFCB777-CAED-42EB-9B0B-CBE135F75017}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15300" windowHeight="7785" xr2:uid="{8FFCB777-CAED-42EB-9B0B-CBE135F75017}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Team</t>
   </si>
@@ -51,14 +51,23 @@
     <t>Team Themba</t>
   </si>
   <si>
-    <t>Team Sbu</t>
+    <t>Team b</t>
+  </si>
+  <si>
+    <t>Team a</t>
+  </si>
+  <si>
+    <t>Team c</t>
+  </si>
+  <si>
+    <t>Team d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +83,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -83,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,14 +121,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,60 +473,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131B74AE-0361-4281-8F46-2B4C27233B06}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>300</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="3">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5">
+        <v>30</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>300</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>300</v>
-      </c>
-      <c r="C4" s="1">
-        <v>13</v>
-      </c>
+      <c r="B5" s="3">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>